<commit_message>
Investing test completed and working
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -87,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +98,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -148,7 +154,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -415,88 +428,88 @@
   <cellXfs count="31">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,7 +858,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="73.15">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="35.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -858,7 +871,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>2</v>

</xml_diff>